<commit_message>
Update Summer 2021 Seed Surveys.xlsx
</commit_message>
<xml_diff>
--- a/Summer Endophyte Surveys/Summer 2021 Seed Surveys.xlsx
+++ b/Summer Endophyte Surveys/Summer 2021 Seed Surveys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicampbell/Box Sync/Grad/Endophytes/2021_summer_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicampbell/Documents/GitHub/Fungal_Endophytes_Summer_2022/Summer Endophyte Surveys/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA700F79-3520-F346-B2E7-5AD36F8E121A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738A7D6F-E406-6B46-A790-A401635D28E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{D98525AB-97B2-884C-9173-2FE30384DD2C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Seed Surveys" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1029,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46714BE-9372-A64A-B392-AF533E4FD8A2}">
   <dimension ref="A1:T152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="O159" sqref="O159"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="R52" sqref="R52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1138,7 +1138,9 @@
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="R2" s="3"/>
+      <c r="R2" s="3">
+        <v>1</v>
+      </c>
       <c r="S2" t="s">
         <v>21</v>
       </c>
@@ -1187,7 +1189,9 @@
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="R3" s="3"/>
+      <c r="R3" s="3">
+        <v>1</v>
+      </c>
       <c r="S3" t="s">
         <v>23</v>
       </c>
@@ -1236,7 +1240,9 @@
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="R4" s="3"/>
+      <c r="R4" s="3">
+        <v>1</v>
+      </c>
       <c r="S4" t="s">
         <v>25</v>
       </c>
@@ -1285,7 +1291,9 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="R5" s="3"/>
+      <c r="R5" s="3">
+        <v>1</v>
+      </c>
       <c r="S5" t="s">
         <v>27</v>
       </c>
@@ -1334,7 +1342,9 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="R6" s="3"/>
+      <c r="R6" s="3">
+        <v>0</v>
+      </c>
       <c r="S6" t="s">
         <v>29</v>
       </c>
@@ -1374,7 +1384,9 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="R7" s="3"/>
+      <c r="R7" s="3">
+        <v>1</v>
+      </c>
       <c r="S7" t="s">
         <v>31</v>
       </c>
@@ -1420,7 +1432,9 @@
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="R8" s="3"/>
+      <c r="R8" s="3">
+        <v>0</v>
+      </c>
       <c r="S8" t="s">
         <v>33</v>
       </c>
@@ -1466,7 +1480,9 @@
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="R9" s="3"/>
+      <c r="R9" s="3">
+        <v>1</v>
+      </c>
       <c r="S9" t="s">
         <v>34</v>
       </c>
@@ -1509,7 +1525,9 @@
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="R10" s="3"/>
+      <c r="R10" s="3">
+        <v>1</v>
+      </c>
       <c r="S10" t="s">
         <v>35</v>
       </c>
@@ -1546,7 +1564,9 @@
       <c r="M11">
         <v>0</v>
       </c>
-      <c r="R11" s="3"/>
+      <c r="R11" s="3">
+        <v>1</v>
+      </c>
       <c r="S11" t="s">
         <v>36</v>
       </c>
@@ -1595,7 +1615,9 @@
       <c r="M12">
         <v>0</v>
       </c>
-      <c r="R12" s="3"/>
+      <c r="R12" s="3">
+        <v>0</v>
+      </c>
       <c r="S12" t="s">
         <v>37</v>
       </c>
@@ -1641,7 +1663,9 @@
       <c r="M13">
         <v>0</v>
       </c>
-      <c r="R13" s="3"/>
+      <c r="R13" s="3">
+        <v>0</v>
+      </c>
       <c r="S13" t="s">
         <v>39</v>
       </c>
@@ -1782,7 +1806,9 @@
       <c r="M16">
         <v>0</v>
       </c>
-      <c r="R16" s="3"/>
+      <c r="R16" s="3">
+        <v>1</v>
+      </c>
       <c r="S16" t="s">
         <v>43</v>
       </c>
@@ -1828,7 +1854,9 @@
       <c r="M17">
         <v>0</v>
       </c>
-      <c r="R17" s="3"/>
+      <c r="R17" s="3">
+        <v>1</v>
+      </c>
       <c r="S17" t="s">
         <v>44</v>
       </c>
@@ -1874,7 +1902,9 @@
       <c r="M18">
         <v>0</v>
       </c>
-      <c r="R18" s="3"/>
+      <c r="R18" s="3">
+        <v>1</v>
+      </c>
       <c r="S18" t="s">
         <v>45</v>
       </c>
@@ -1911,7 +1941,9 @@
       <c r="M19">
         <v>0</v>
       </c>
-      <c r="R19" s="3"/>
+      <c r="R19" s="3">
+        <v>1</v>
+      </c>
       <c r="S19" t="s">
         <v>46</v>
       </c>
@@ -1960,7 +1992,9 @@
       <c r="M20">
         <v>0</v>
       </c>
-      <c r="R20" s="3"/>
+      <c r="R20" s="3">
+        <v>0</v>
+      </c>
       <c r="S20" t="s">
         <v>47</v>
       </c>
@@ -1997,7 +2031,9 @@
       <c r="M21">
         <v>0</v>
       </c>
-      <c r="R21" s="3"/>
+      <c r="R21" s="3">
+        <v>0</v>
+      </c>
       <c r="S21" t="s">
         <v>48</v>
       </c>
@@ -2046,7 +2082,9 @@
       <c r="M22">
         <v>0</v>
       </c>
-      <c r="R22" s="3"/>
+      <c r="R22" s="3">
+        <v>0</v>
+      </c>
       <c r="S22" t="s">
         <v>49</v>
       </c>
@@ -2092,7 +2130,9 @@
       <c r="M23">
         <v>0</v>
       </c>
-      <c r="R23" s="3"/>
+      <c r="R23" s="3">
+        <v>1</v>
+      </c>
       <c r="S23" t="s">
         <v>50</v>
       </c>
@@ -2129,7 +2169,9 @@
       <c r="M24">
         <v>0</v>
       </c>
-      <c r="R24" s="3"/>
+      <c r="R24" s="3">
+        <v>0</v>
+      </c>
       <c r="S24" t="s">
         <v>51</v>
       </c>
@@ -2169,7 +2211,9 @@
       <c r="M25">
         <v>0</v>
       </c>
-      <c r="R25" s="3"/>
+      <c r="R25" s="3">
+        <v>1</v>
+      </c>
       <c r="S25" t="s">
         <v>52</v>
       </c>
@@ -2209,7 +2253,9 @@
       <c r="M26">
         <v>0</v>
       </c>
-      <c r="R26" s="3"/>
+      <c r="R26" s="3">
+        <v>0</v>
+      </c>
       <c r="S26" t="s">
         <v>53</v>
       </c>
@@ -2258,7 +2304,9 @@
       <c r="M27">
         <v>0</v>
       </c>
-      <c r="R27" s="3"/>
+      <c r="R27" s="3">
+        <v>0</v>
+      </c>
       <c r="S27" t="s">
         <v>54</v>
       </c>
@@ -2390,7 +2438,9 @@
       <c r="M30">
         <v>0</v>
       </c>
-      <c r="R30" s="3"/>
+      <c r="R30" s="3">
+        <v>0</v>
+      </c>
       <c r="S30" t="s">
         <v>57</v>
       </c>
@@ -2427,7 +2477,9 @@
       <c r="M31">
         <v>0</v>
       </c>
-      <c r="R31" s="3"/>
+      <c r="R31" s="3">
+        <v>1</v>
+      </c>
       <c r="S31" t="s">
         <v>58</v>
       </c>
@@ -2467,7 +2519,9 @@
       <c r="M32">
         <v>0</v>
       </c>
-      <c r="R32" s="3"/>
+      <c r="R32" s="3">
+        <v>1</v>
+      </c>
       <c r="S32" t="s">
         <v>59</v>
       </c>
@@ -2507,7 +2561,9 @@
       <c r="M33">
         <v>0</v>
       </c>
-      <c r="R33" s="3"/>
+      <c r="R33" s="3">
+        <v>0</v>
+      </c>
       <c r="S33" t="s">
         <v>60</v>
       </c>
@@ -2547,7 +2603,9 @@
       <c r="M34">
         <v>0</v>
       </c>
-      <c r="R34" s="3"/>
+      <c r="R34" s="3">
+        <v>1</v>
+      </c>
       <c r="S34" t="s">
         <v>61</v>
       </c>
@@ -2587,7 +2645,9 @@
       <c r="M35">
         <v>0</v>
       </c>
-      <c r="R35" s="3"/>
+      <c r="R35" s="3">
+        <v>1</v>
+      </c>
       <c r="S35" t="s">
         <v>62</v>
       </c>
@@ -2633,7 +2693,9 @@
       <c r="M36">
         <v>0</v>
       </c>
-      <c r="R36" s="3"/>
+      <c r="R36" s="3">
+        <v>0</v>
+      </c>
       <c r="S36" t="s">
         <v>63</v>
       </c>
@@ -2676,7 +2738,9 @@
       <c r="M37">
         <v>0</v>
       </c>
-      <c r="R37" s="3"/>
+      <c r="R37" s="3">
+        <v>0</v>
+      </c>
       <c r="S37" t="s">
         <v>64</v>
       </c>
@@ -2719,7 +2783,9 @@
       <c r="M38">
         <v>0</v>
       </c>
-      <c r="R38" s="3"/>
+      <c r="R38" s="3">
+        <v>1</v>
+      </c>
       <c r="S38" t="s">
         <v>65</v>
       </c>
@@ -2762,7 +2828,9 @@
       <c r="M39">
         <v>0</v>
       </c>
-      <c r="R39" s="3"/>
+      <c r="R39" s="3">
+        <v>1</v>
+      </c>
       <c r="S39" t="s">
         <v>66</v>
       </c>
@@ -2802,7 +2870,9 @@
       <c r="M40">
         <v>0</v>
       </c>
-      <c r="R40" s="3"/>
+      <c r="R40" s="3">
+        <v>0</v>
+      </c>
       <c r="S40" t="s">
         <v>67</v>
       </c>
@@ -2842,7 +2912,9 @@
       <c r="M41">
         <v>0</v>
       </c>
-      <c r="R41" s="3"/>
+      <c r="R41" s="3">
+        <v>1</v>
+      </c>
       <c r="S41" t="s">
         <v>68</v>
       </c>
@@ -2922,7 +2994,6 @@
       <c r="M43">
         <v>0</v>
       </c>
-      <c r="R43" s="3"/>
       <c r="S43" t="s">
         <v>70</v>
       </c>
@@ -2968,7 +3039,9 @@
       <c r="M44">
         <v>0</v>
       </c>
-      <c r="R44" s="3"/>
+      <c r="R44" s="3">
+        <v>0</v>
+      </c>
       <c r="S44" t="s">
         <v>71</v>
       </c>
@@ -3005,7 +3078,9 @@
       <c r="M45">
         <v>0</v>
       </c>
-      <c r="R45" s="3"/>
+      <c r="R45" s="3">
+        <v>1</v>
+      </c>
       <c r="S45" t="s">
         <v>72</v>
       </c>
@@ -3042,7 +3117,9 @@
       <c r="M46">
         <v>0</v>
       </c>
-      <c r="R46" s="3"/>
+      <c r="R46" s="3">
+        <v>1</v>
+      </c>
       <c r="S46" t="s">
         <v>73</v>
       </c>
@@ -3082,7 +3159,9 @@
       <c r="M47">
         <v>0</v>
       </c>
-      <c r="R47" s="3"/>
+      <c r="R47" s="3">
+        <v>0</v>
+      </c>
       <c r="S47" t="s">
         <v>74</v>
       </c>
@@ -3122,7 +3201,9 @@
       <c r="M48">
         <v>0</v>
       </c>
-      <c r="R48" s="3"/>
+      <c r="R48" s="3">
+        <v>1</v>
+      </c>
       <c r="S48" t="s">
         <v>75</v>
       </c>
@@ -3168,7 +3249,9 @@
       <c r="M49">
         <v>0</v>
       </c>
-      <c r="R49" s="3"/>
+      <c r="R49" s="3">
+        <v>0</v>
+      </c>
       <c r="S49" t="s">
         <v>76</v>
       </c>
@@ -3205,7 +3288,9 @@
       <c r="M50">
         <v>0</v>
       </c>
-      <c r="R50" s="3"/>
+      <c r="R50" s="3">
+        <v>0</v>
+      </c>
       <c r="S50" t="s">
         <v>77</v>
       </c>
@@ -3245,7 +3330,9 @@
       <c r="M51">
         <v>0</v>
       </c>
-      <c r="R51" s="3"/>
+      <c r="R51" s="3">
+        <v>1</v>
+      </c>
       <c r="S51" t="s">
         <v>78</v>
       </c>

</xml_diff>